<commit_message>
Modelo físico banco de dados adicionado, Context e CRUD de Aluno criado
</commit_message>
<xml_diff>
--- a/ModelagemBancoDeDados/ModeloFisico.xlsx
+++ b/ModelagemBancoDeDados/ModeloFisico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrodr.LAPTOP-DFNK1JF6\Desktop\DesafioMarlin\ModelagemBancoDeDados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus\Desktop\desafio-marvin\ModelagemBancoDeDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF6F02F0-D659-4199-8FCE-2AE0A8CFFCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277DEB67-456D-4F53-A5F3-E63A123420CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFD9A8FD-1703-4391-B9C5-C04C3ADCE7C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFD9A8FD-1703-4391-B9C5-C04C3ADCE7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Alunos</t>
   </si>
@@ -133,7 +133,94 @@
     <t>João Soares</t>
   </si>
   <si>
-    <t xml:space="preserve">Maria </t>
+    <t>Maria Silva</t>
+  </si>
+  <si>
+    <t>carlostsuka@email.com</t>
+  </si>
+  <si>
+    <t>joao@email.com</t>
+  </si>
+  <si>
+    <t>maria@email.com</t>
+  </si>
+  <si>
+    <t>197d2787-fec6-e830-e6ed-f6740137b5df</t>
+  </si>
+  <si>
+    <t>c2ebed27-6196-596c-4b19-607239873f0c</t>
+  </si>
+  <si>
+    <t>0e2619ea-5742-f5d5-4237-953960134115</t>
+  </si>
+  <si>
+    <t>7a92ed4b-28db-8d17-b9d7-e13f7484f5f8</t>
+  </si>
+  <si>
+    <t>319d7165-c5ce-be50-4171-674c26c2f0d6</t>
+  </si>
+  <si>
+    <t>Leonardo Costa</t>
+  </si>
+  <si>
+    <t>Miguel Melo</t>
+  </si>
+  <si>
+    <t>Murilo Silva</t>
+  </si>
+  <si>
+    <t>miguel@email.com</t>
+  </si>
+  <si>
+    <t>murilo@email.com</t>
+  </si>
+  <si>
+    <t>leonardo@email.com</t>
+  </si>
+  <si>
+    <t>descricaoTurma</t>
+  </si>
+  <si>
+    <t>Inglês</t>
+  </si>
+  <si>
+    <t>Alemão</t>
+  </si>
+  <si>
+    <t>Espanhol</t>
+  </si>
+  <si>
+    <t>c7f40b10-97e6-43d3-1301-260b07efe4ad</t>
+  </si>
+  <si>
+    <t>dec107b4-6318-46f0-c94a-71ca5dc93e8f</t>
+  </si>
+  <si>
+    <t>86f59797-1e3a-b243-17fd-2f1c1d2e08d5</t>
+  </si>
+  <si>
+    <t>6bf3c714-8a7a-82e1-240c-42621450e735</t>
+  </si>
+  <si>
+    <t>c80ad692-a67a-a9f0-9c85-a6927583962e</t>
+  </si>
+  <si>
+    <t>eb9c984c-af29-7c7a-f7dc-a8b482a204b2</t>
+  </si>
+  <si>
+    <t>283fa435-97cd-b843-3570-9f0540c41036</t>
+  </si>
+  <si>
+    <t>59240eb2-45a8-9638-4f24-e80e94da84d5</t>
+  </si>
+  <si>
+    <t>b6ae0d0a-2645-e71b-a567-b1c6a6a35b40</t>
+  </si>
+  <si>
+    <t>73fbd9d6-4154-1639-e4de-23c5fad93484</t>
+  </si>
+  <si>
+    <t>ba0aef92-71f9-73ab-13a5-64d9dbf76df4</t>
   </si>
 </sst>
 </file>
@@ -157,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +266,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,20 +328,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -540,239 +675,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99446AC-774E-498D-B0B5-7ED00DBFB1C3}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>12345678999</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="9">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="9">
         <v>2022</v>
       </c>
-      <c r="L3" t="s">
+      <c r="J3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>49278288080</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="9">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="9">
         <v>2023</v>
       </c>
-      <c r="L4" t="s">
+      <c r="J4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>68098450031</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="9">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="9">
         <v>2024</v>
       </c>
-      <c r="L5" t="s">
+      <c r="J5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>69025933025</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M6" t="s">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3">
+        <v>24197333048</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5">
-        <v>24197333048</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>80106940023</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="C9" s="3">
+        <v>26536869028</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="3">
+        <v>49996230058</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3">
+        <v>55020770043</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3">
+        <v>79042131098</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="11">
+        <v>57591643045</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:M1"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{42C69309-0ECF-4C87-8176-75B30B456330}"/>
@@ -781,6 +1054,11 @@
     <hyperlink ref="D6" r:id="rId4" xr:uid="{0A85C005-215C-40A7-A8AD-7826444CE145}"/>
     <hyperlink ref="D7" r:id="rId5" xr:uid="{EB9B8674-1C3E-42D7-ABDF-77F8A522F8AD}"/>
     <hyperlink ref="D8" r:id="rId6" xr:uid="{4A70D3DD-BB1E-4BF3-95BB-1C45172D77C4}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{0443FF59-76F4-4542-829F-B49EAEADF0D2}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{E42D7820-181A-425E-B194-63709177F538}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{B09E5ED1-9CE0-49D4-83C9-80E31B43589D}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{69D47B5A-9EAF-43D4-9249-F42022A1DC4B}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{B288E9B7-97BF-40DA-9101-6126E60F1E69}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>